<commit_message>
Uploaded revised RTM for March 2017 CDP
</commit_message>
<xml_diff>
--- a/Documentation/Monthly Deliverables/RTM/BCDSS_RTM_03_22_2017.xlsx
+++ b/Documentation/Monthly Deliverables/RTM/BCDSS_RTM_03_22_2017.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\BCDS\RTM BCDS\RTM March 2017\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ganesh Panneer\Project Documents\BCDSS\Documents\Collabrative Dev_Package\March 2017\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9090" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Legend" sheetId="1" r:id="rId1"/>
@@ -23,8 +23,8 @@
   </definedNames>
   <calcPr calcId="152511"/>
   <customWorkbookViews>
+    <customWorkbookView name="Ganesh Panneer - Personal View" guid="{64356ACC-46E0-4594-A667-8B3867E089EA}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="2"/>
     <customWorkbookView name="Evan Weber - Personal View" guid="{265E3820-1829-4A54-B10C-5E3DB0A2FE40}" mergeInterval="0" personalView="1" maximized="1" xWindow="-9" yWindow="-9" windowWidth="1698" windowHeight="1020" activeSheetId="2"/>
-    <customWorkbookView name="Ganesh Panneer - Personal View" guid="{64356ACC-46E0-4594-A667-8B3867E089EA}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="2"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -1125,35 +1125,6 @@
     <t xml:space="preserve">Wireframe: Modeling Agent Dashboard </t>
   </si>
   <si>
-    <t xml:space="preserve">As a Rater, I need to be able to search a specific claim or set of claims from the sample data provided, so that I can run the predictive model for that specific claim(s)._x000D_
-_x000D_
-Assumption: The user is aware of the claim(s) available in the sample claims provided._x000D_
-_x000D_
-Acceptance Criteria: The search must return the claims based on the entered search criteria._x000D_
-_x000D_
-Note:_x000D_
-Mockup of the "Advanced Filter" Pop-up attached._x000D_
-_x000D_
-Details of the steps_x000D_
-_x000D_
-1.      Select "Advanced Search" from the Rater/Modelling Agent Dashboard_x000D_
-2.      â€œAdvance Filterâ€ pop-up is displayed_x000D_
-a.      Select â€œDate of Claimâ€ or â€œClaim Established dateâ€ by selecting the radio button (they are mutually exclusive items and mandatory)_x000D_
-b.      Enter â€œFromâ€ date (mandatory field)_x000D_
-c.      Enter â€œtoâ€ date (mandatory field)_x000D_
-d.      Enter â€œContentionâ€ text (Optional field)_x000D_
-e.      Enter â€œRegional Officeâ€ dropdown (Optional field)_x000D_
-f.       Click â€œFilterâ€ â€“ Shall skip to the dashboard with the filtered claims displayed on the Dashboard_x000D_
-g.      Click â€œCancelâ€ shall skip to the Dashboard without filtering_x000D_
-_x000D_
-_x000D_
-Also  there must be warning message if " from date' value   is entered  after  "to date"_x000D_
-_x000D_
-Regional Data in dropdown box should show alphabetically_x000D_
-_x000D_
-</t>
-  </si>
-  <si>
     <t>As a developer, I want to data objects for claims page so that target claim data from bcdss database</t>
   </si>
   <si>
@@ -1270,27 +1241,6 @@
     <t>BCDS - Results page updates for the Processed Contentions</t>
   </si>
   <si>
-    <t xml:space="preserve">As a Rater, I need to view the output of the Predictive Model, so that I can compare it with the actual Rating output._x000D_
-_x000D_
-Assumption: Predictive models are available and able to successfully process the contention._x000D_
-_x000D_
-Acceptance Criteria: There is a compensation assigned to the processed contention._x000D_
-_x000D_
-Note:_x000D_
-a. The Column description should be displayed when the user hover over the column headers_x000D_
-       Field names and description is pasted in the comment section _x000D_
-b. When clicked on the Model Result ID display the Detailed Report contents, and Narrative (recommendation) to Rater along with appropriate recommendation based on the Ranges for  "pattern accuracy" (listed below)_x000D_
-_x000D_
-Narrative with variables in bold text_x000D_
-The fact pattern used to statistically determine the rating for the target issue/issues has proven to be *SOMEWHAT RELIABLE* based on the frequency with which the same facts have been presented to support a supplemental claim for increase, and the number of times the same rating has been determined by VBA RVSRs. Â The calculated confidence level - based on a population size of *50 EAR* related claims over the past 10 years - *EXCEEDS 98%*._x000D_
-_x000D_
-Ranges for the pattern accuracy and recommendation are as following_x000D_
-1.Â Â Â Â  If the pattern accuracy Exceeds 99.5% - itâ€™s considered â€˜Extremely Reliableâ€™._x000D_
-2.Â Â Â Â  If the pattern accuracy is between 98.5% and 99.49% - itâ€™s considered â€˜Very Reliableâ€™._x000D_
-3.Â Â Â Â  If the pattern accuracy is between 90% and 98.49% - itâ€™s considered 'Somewhat Reliableâ€™._x000D_
-4.Â Â Â Â  If the pattern accuracy is less than 90% - itâ€™s considered 'Not Reliableâ€™. </t>
-  </si>
-  <si>
     <t>VABCDS-201</t>
   </si>
   <si>
@@ -1422,22 +1372,6 @@
   </si>
   <si>
     <t>VABCDS-831</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As a Rater, I want to be able to Agree/Disagree the Model generated results, so that I can provide my inputs on the model results._x000D_
-_x000D_
-*Note:*_x000D_
-Changes as discussed on 12/27/2016 with the team internally_x000D_
-â€¢	Add an additional column as â€œStatusâ€ before column â€œAgree (Y/N)â€_x000D_
-â€¢	Status â€“ Previous (from the most recent) status of the claim as per Rater/System.  Will have 3 status as - Agreed/Disagreed/Processed. It's a read only field (no user action). _x000D_
-â€¢	Column â€œAgree (Y/N)â€ will be made as a drop down menu with 2 options as â€“ Agree &amp; Disagree (for Model Results that Rater is unable to make decision).  The selected value will be retrieved in the â€œStatusâ€ column when the claim is searched or processed at a later time._x000D_
-_x000D_
-_x000D_
-â€¢      "Save" button - When the Rater clicks the save button all user action should be recorded in the Result Status table. i.e. the rater who processed the claim, Agree(Y/N) updates._x000D_
-â€¢       Leave the "Reason" as null on the Result Status table_x000D_
-_x000D_
-Any questions/clarification please contact CJ/Vasu_x000D_
-</t>
   </si>
   <si>
     <t>VABCDS-828</t>
@@ -1492,36 +1426,6 @@
     <t>BCDS - Rater: Produce Analysis Reports for each Rated Contention</t>
   </si>
   <si>
-    <t xml:space="preserve">As a Rater, I need the system to have the capability to produce report for viewing for each rated contention with the details of analysis how the BCDS system recommended rating was achieved and all the relevant supporting information, so that I can understand and validate the model rating produced by BCDSS._x000D_
-_x000D_
-Assumption:_x000D_
-# The Rater is successfully logged into the system._x000D_
-# The system has successfully processed contentions of the claims._x000D_
-_x000D_
-Acceptance Criteria:_x000D_
-# The system will generate a report for each rated contention with the analysis details of how the rating was determined by the models for each contention._x000D_
-# The generated report should be made available to the Rater._x000D_
-# The Rater should be able to save the report_x000D_
-# The report should be in a format that could potentially be uploaded to the Veteran's eFolder._x000D_
-_x000D_
-*Steps to get Analysis Reports for Rater*_x000D_
-When the Rater clicks the report tab_x000D_
-a)	Navigate to the Reports page _x000D_
-b)	Enter Search criteria (refer attached â€œRater Homeâ€ mockup screen)_x000D_
-        Note: One or more search criteria required to get the desired report_x000D_
-   i)	   Enter â€œClaim Processing dateâ€ range (Max one year date range allowed) (Optional)_x000D_
-   ii)	   Select â€œModelâ€ from the dropdown (Optional)_x000D_
-   iii)	   OR Enter â€œModel Result IDâ€ (Optional)_x000D_
-   iv)	   Select â€œReport Typeâ€ generate the Detailed Report (Mandatory field). Keep this as a dropdown for any future report request from client_x000D_
-   v)	   Select â€œOutput typeâ€ to generate the report in that format (Mandatory field) - HTML or PDF file._x000D_
-   vi)	   Click â€œGenerate Reportâ€ button_x000D_
-c)	The new window will open in the selected â€œOutput typeâ€ format_x000D_
-d)	Save the generated report to local system_x000D_
-_x000D_
-_x000D_
-</t>
-  </si>
-  <si>
     <t>VABCDS-549</t>
   </si>
   <si>
@@ -1603,6 +1507,102 @@
   </si>
   <si>
     <t>VABCDS-955</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a Rater, I want to be able to Agree/Disagree the Model generated results, so that I can provide my inputs on the model results._x000D_
+_x000D_
+*Note:*_x000D_
+Changes as discussed on 12/27/2016 with the team internally_x000D_
+"¢	Add an additional column as "Status" before column "Agree (Y/N)"_x000D_
+"¢	Status "“ Previous (from the most recent) status of the claim as per Rater/System.  Will have 3 status as - Agreed/Disagreed/Processed. It's a read only field (no user action). _x000D_
+"¢	Column "Agree (Y/N)" will be made as a drop down menu with 2 options as "“ Agree &amp; Disagree (for Model Results that Rater is unable to make decision).  The selected value will be retrieved in the "Status" column when the claim is searched or processed at a later time._x000D_
+_x000D_
+_x000D_
+"¢      "Save" button - When the Rater clicks the save button all user action should be recorded in the Result Status table. i.e. the rater who processed the claim, Agree(Y/N) updates._x000D_
+"¢       Leave the "Reason" as null on the Result Status table_x000D_
+_x000D_
+Any questions/clarification please contact CJ/Vasu_x000D_
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a Rater, I need to view the output of the Predictive Model, so that I can compare it with the actual Rating output._x000D_
+_x000D_
+Assumption: Predictive models are available and able to successfully process the contention._x000D_
+_x000D_
+Acceptance Criteria: There is a compensation assigned to the processed contention._x000D_
+_x000D_
+Note:_x000D_
+a. The Column description should be displayed when the user hover over the column headers_x000D_
+       Field names and description is pasted in the comment section _x000D_
+b. When clicked on the Model Result ID display the Detailed Report contents, and Narrative (recommendation) to Rater along with appropriate recommendation based on the Ranges for  "pattern accuracy" (listed below)_x000D_
+_x000D_
+Narrative with variables in bold text_x000D_
+The fact pattern used to statistically determine the rating for the target issue/issues has proven to be *SOMEWHAT RELIABLE* based on the frequency with which the same facts have been presented to support a supplemental claim for increase, and the number of times the same rating has been determined by VBA RVSRs. Â The calculated confidence level - based on a population size of *50 EAR* related claims over the past 10 years - *EXCEEDS 98%*._x000D_
+_x000D_
+Ranges for the pattern accuracy and recommendation are as following_x000D_
+1.Â Â Â Â  If the pattern accuracy Exceeds 99.5% - it"™s considered "˜Extremely Reliable"™._x000D_
+2.Â Â Â Â  If the pattern accuracy is between 98.5% and 99.49% - it"™s considered "˜Very Reliable"™._x000D_
+3.Â Â Â Â  If the pattern accuracy is between 90% and 98.49% - it"™s considered 'Somewhat Reliable"™._x000D_
+4.Â Â Â Â  If the pattern accuracy is less than 90% - it"™s considered 'Not Reliable"™. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a Rater, I need the system to have the capability to produce report for viewing for each rated contention with the details of analysis how the BCDS system recommended rating was achieved and all the relevant supporting information, so that I can understand and validate the model rating produced by BCDSS._x000D_
+_x000D_
+Assumption:_x000D_
+# The Rater is successfully logged into the system._x000D_
+# The system has successfully processed contentions of the claims._x000D_
+_x000D_
+Acceptance Criteria:_x000D_
+# The system will generate a report for each rated contention with the analysis details of how the rating was determined by the models for each contention._x000D_
+# The generated report should be made available to the Rater._x000D_
+# The Rater should be able to save the report_x000D_
+# The report should be in a format that could potentially be uploaded to the Veteran's eFolder._x000D_
+_x000D_
+*Steps to get Analysis Reports for Rater*_x000D_
+When the Rater clicks the report tab_x000D_
+a)	Navigate to the Reports page _x000D_
+b)	Enter Search criteria (refer attached "Rater Home" mockup screen)_x000D_
+        Note: One or more search criteria required to get the desired report_x000D_
+   i)	   Enter "Claim Processing date" range (Max one year date range allowed) (Optional)_x000D_
+   ii)	   Select "Model" from the dropdown (Optional)_x000D_
+   iii)	   OR Enter "Model Result ID" (Optional)_x000D_
+   iv)	   Select "Report Type" generate the Detailed Report (Mandatory field). Keep this as a dropdown for any future report request from client_x000D_
+   v)	   Select "Output type" to generate the report in that format (Mandatory field) - HTML or PDF file._x000D_
+   vi)	   Click "Generate Report" button_x000D_
+c)	The new window will open in the selected "Output type" format_x000D_
+d)	Save the generated report to local system_x000D_
+_x000D_
+_x000D_
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a Rater, I need to be able to search a specific claim or set of claims from the sample data provided, so that I can run the predictive model for that specific claim(s)._x000D_
+_x000D_
+Assumption: The user is aware of the claim(s) available in the sample claims provided._x000D_
+_x000D_
+Acceptance Criteria: The search must return the claims based on the entered search criteria._x000D_
+_x000D_
+Note:_x000D_
+Mockup of the "Advanced Filter" Pop-up attached._x000D_
+_x000D_
+Details of the steps_x000D_
+_x000D_
+1.      Select "Advanced Search" from the Rater/Modelling Agent Dashboard_x000D_
+2.      "Advance Filter" pop-up is displayed_x000D_
+a.      Select "Date of Claim" or "Claim Established date" by selecting the radio button (they are mutually exclusive items and mandatory)_x000D_
+b.      Enter "From" date (mandatory field)_x000D_
+c.      Enter "to" date (mandatory field)_x000D_
+d.      Enter "Contention" text (Optional field)_x000D_
+e.      Enter "Regional Office" dropdown (Optional field)_x000D_
+f.       Click "Filter" Shall skip to the dashboard with the filtered claims displayed on the Dashboard_x000D_
+g.      Click "Cancel" shall skip to the Dashboard without filtering_x000D_
+_x000D_
+_x000D_
+Also  there must be warning message if " from date' value   is entered  after  "to date"_x000D_
+_x000D_
+Regional Data in dropdown box should show alphabetically_x000D_
+_x000D_
+</t>
   </si>
 </sst>
 </file>
@@ -2379,18 +2379,54 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -2399,42 +2435,6 @@
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="20" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -2880,12 +2880,12 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{265E3820-1829-4A54-B10C-5E3DB0A2FE40}">
+    <customSheetView guid="{64356ACC-46E0-4594-A667-8B3867E089EA}">
       <selection activeCell="B2" sqref="B2"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{64356ACC-46E0-4594-A667-8B3867E089EA}">
+    <customSheetView guid="{265E3820-1829-4A54-B10C-5E3DB0A2FE40}">
       <selection activeCell="B2" sqref="B2"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId2"/>
@@ -2905,9 +2905,9 @@
   <dimension ref="A1:I109"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="140" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A107" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="2" topLeftCell="A105" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="C115" sqref="C115"/>
+      <selection pane="bottomLeft" activeCell="H28" sqref="H28:H53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -2925,16 +2925,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="43" t="s">
         <v>121</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
-      <c r="F1" s="59"/>
-      <c r="G1" s="59"/>
-      <c r="H1" s="59"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
     </row>
     <row r="2" spans="1:9" s="1" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
@@ -2964,16 +2964,16 @@
       <c r="I2" s="5"/>
     </row>
     <row r="3" spans="1:9" s="9" customFormat="1" ht="156.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="41" t="s">
+      <c r="A3" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="43" t="s">
+      <c r="B3" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="41" t="s">
+      <c r="C3" s="44" t="s">
         <v>122</v>
       </c>
-      <c r="D3" s="43" t="s">
+      <c r="D3" s="47" t="s">
         <v>73</v>
       </c>
       <c r="E3" s="36"/>
@@ -2989,52 +2989,52 @@
       <c r="I3" s="8"/>
     </row>
     <row r="4" spans="1:9" s="9" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="42"/>
-      <c r="B4" s="44"/>
-      <c r="C4" s="42"/>
-      <c r="D4" s="44"/>
+      <c r="A4" s="45"/>
+      <c r="B4" s="48"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="48"/>
       <c r="E4" s="17" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="F4" s="17" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="G4" s="17" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="H4" s="36"/>
       <c r="I4" s="8"/>
     </row>
     <row r="5" spans="1:9" s="9" customFormat="1" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="42"/>
-      <c r="B5" s="44"/>
-      <c r="C5" s="42"/>
-      <c r="D5" s="44"/>
+      <c r="A5" s="45"/>
+      <c r="B5" s="48"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="48"/>
       <c r="E5" s="17" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="F5" s="17" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="G5" s="17" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="H5" s="36"/>
       <c r="I5" s="8"/>
     </row>
     <row r="6" spans="1:9" s="9" customFormat="1" ht="256.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="49"/>
-      <c r="B6" s="48"/>
-      <c r="C6" s="49"/>
-      <c r="D6" s="48"/>
+      <c r="A6" s="46"/>
+      <c r="B6" s="49"/>
+      <c r="C6" s="46"/>
+      <c r="D6" s="49"/>
       <c r="E6" s="17" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="F6" s="17" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="G6" s="17" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="H6" s="39"/>
       <c r="I6" s="8"/>
@@ -3049,7 +3049,7 @@
       <c r="C7" s="51" t="s">
         <v>123</v>
       </c>
-      <c r="D7" s="43" t="s">
+      <c r="D7" s="47" t="s">
         <v>49</v>
       </c>
       <c r="E7" s="21" t="s">
@@ -3070,7 +3070,7 @@
       <c r="A8" s="50"/>
       <c r="B8" s="50"/>
       <c r="C8" s="51"/>
-      <c r="D8" s="44"/>
+      <c r="D8" s="48"/>
       <c r="E8" s="21" t="s">
         <v>112</v>
       </c>
@@ -3087,7 +3087,7 @@
       <c r="A9" s="50"/>
       <c r="B9" s="50"/>
       <c r="C9" s="51"/>
-      <c r="D9" s="44"/>
+      <c r="D9" s="48"/>
       <c r="E9" s="22" t="s">
         <v>292</v>
       </c>
@@ -3104,7 +3104,7 @@
       <c r="A10" s="50"/>
       <c r="B10" s="50"/>
       <c r="C10" s="51"/>
-      <c r="D10" s="44"/>
+      <c r="D10" s="48"/>
       <c r="E10" s="21" t="s">
         <v>114</v>
       </c>
@@ -3121,7 +3121,7 @@
       <c r="A11" s="50"/>
       <c r="B11" s="50"/>
       <c r="C11" s="51"/>
-      <c r="D11" s="44"/>
+      <c r="D11" s="48"/>
       <c r="E11" s="21" t="s">
         <v>116</v>
       </c>
@@ -3319,13 +3319,13 @@
       <c r="I21" s="8"/>
     </row>
     <row r="22" spans="1:9" s="9" customFormat="1" ht="171" x14ac:dyDescent="0.25">
-      <c r="A22" s="43" t="s">
+      <c r="A22" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="B22" s="43" t="s">
+      <c r="B22" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="C22" s="41" t="s">
+      <c r="C22" s="44" t="s">
         <v>101</v>
       </c>
       <c r="D22" s="50" t="s">
@@ -3346,9 +3346,9 @@
       <c r="I22" s="8"/>
     </row>
     <row r="23" spans="1:9" s="9" customFormat="1" ht="128.25" x14ac:dyDescent="0.25">
-      <c r="A23" s="44"/>
-      <c r="B23" s="44"/>
-      <c r="C23" s="42"/>
+      <c r="A23" s="48"/>
+      <c r="B23" s="48"/>
+      <c r="C23" s="45"/>
       <c r="D23" s="50"/>
       <c r="E23" s="17" t="s">
         <v>66</v>
@@ -3365,64 +3365,64 @@
       <c r="I23" s="8"/>
     </row>
     <row r="24" spans="1:9" s="9" customFormat="1" ht="185.25" x14ac:dyDescent="0.25">
-      <c r="A24" s="44"/>
-      <c r="B24" s="44"/>
-      <c r="C24" s="42"/>
-      <c r="D24" s="52" t="s">
-        <v>385</v>
+      <c r="A24" s="48"/>
+      <c r="B24" s="48"/>
+      <c r="C24" s="45"/>
+      <c r="D24" s="56" t="s">
+        <v>381</v>
       </c>
       <c r="E24" s="17" t="s">
         <v>224</v>
       </c>
       <c r="F24" s="17" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="G24" s="17" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="H24" s="27"/>
       <c r="I24" s="8"/>
     </row>
     <row r="25" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="44"/>
-      <c r="B25" s="44"/>
-      <c r="C25" s="42"/>
-      <c r="D25" s="52"/>
+      <c r="A25" s="48"/>
+      <c r="B25" s="48"/>
+      <c r="C25" s="45"/>
+      <c r="D25" s="56"/>
       <c r="E25" s="17" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="F25" s="17" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="G25" s="17"/>
       <c r="H25" s="27"/>
       <c r="I25" s="8"/>
     </row>
     <row r="26" spans="1:9" s="9" customFormat="1" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="44"/>
-      <c r="B26" s="44"/>
-      <c r="C26" s="42"/>
-      <c r="D26" s="52"/>
+      <c r="A26" s="48"/>
+      <c r="B26" s="48"/>
+      <c r="C26" s="45"/>
+      <c r="D26" s="56"/>
       <c r="E26" s="17" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="F26" s="17" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="G26" s="17"/>
       <c r="H26" s="27"/>
       <c r="I26" s="8"/>
     </row>
     <row r="27" spans="1:9" s="9" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A27" s="48"/>
-      <c r="B27" s="48"/>
-      <c r="C27" s="49"/>
-      <c r="D27" s="52"/>
+      <c r="A27" s="49"/>
+      <c r="B27" s="49"/>
+      <c r="C27" s="46"/>
+      <c r="D27" s="56"/>
       <c r="E27" s="17" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="F27" s="17" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="G27" s="17"/>
       <c r="H27" s="27"/>
@@ -3438,7 +3438,7 @@
       <c r="C28" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="D28" s="43" t="s">
+      <c r="D28" s="47" t="s">
         <v>51</v>
       </c>
       <c r="E28" s="22" t="s">
@@ -3450,7 +3450,7 @@
       <c r="G28" s="22" t="s">
         <v>297</v>
       </c>
-      <c r="H28" s="41" t="s">
+      <c r="H28" s="44" t="s">
         <v>82</v>
       </c>
       <c r="I28" s="8"/>
@@ -3459,7 +3459,7 @@
       <c r="A29" s="50"/>
       <c r="B29" s="50"/>
       <c r="C29" s="51"/>
-      <c r="D29" s="44"/>
+      <c r="D29" s="48"/>
       <c r="E29" s="22" t="s">
         <v>163</v>
       </c>
@@ -3469,14 +3469,14 @@
       <c r="G29" s="22" t="s">
         <v>298</v>
       </c>
-      <c r="H29" s="42"/>
+      <c r="H29" s="45"/>
       <c r="I29" s="8"/>
     </row>
     <row r="30" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="50"/>
       <c r="B30" s="50"/>
       <c r="C30" s="51"/>
-      <c r="D30" s="44"/>
+      <c r="D30" s="48"/>
       <c r="E30" s="22" t="s">
         <v>165</v>
       </c>
@@ -3486,14 +3486,14 @@
       <c r="G30" s="22" t="s">
         <v>166</v>
       </c>
-      <c r="H30" s="42"/>
+      <c r="H30" s="45"/>
       <c r="I30" s="8"/>
     </row>
     <row r="31" spans="1:9" s="9" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A31" s="50"/>
       <c r="B31" s="50"/>
       <c r="C31" s="51"/>
-      <c r="D31" s="44"/>
+      <c r="D31" s="48"/>
       <c r="E31" s="22" t="s">
         <v>167</v>
       </c>
@@ -3503,14 +3503,14 @@
       <c r="G31" s="22" t="s">
         <v>168</v>
       </c>
-      <c r="H31" s="42"/>
+      <c r="H31" s="45"/>
       <c r="I31" s="8"/>
     </row>
     <row r="32" spans="1:9" s="9" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A32" s="50"/>
       <c r="B32" s="50"/>
       <c r="C32" s="51"/>
-      <c r="D32" s="44"/>
+      <c r="D32" s="48"/>
       <c r="E32" s="22" t="s">
         <v>169</v>
       </c>
@@ -3518,16 +3518,16 @@
         <v>170</v>
       </c>
       <c r="G32" s="22" t="s">
-        <v>301</v>
-      </c>
-      <c r="H32" s="42"/>
+        <v>389</v>
+      </c>
+      <c r="H32" s="45"/>
       <c r="I32" s="8"/>
     </row>
     <row r="33" spans="1:9" s="9" customFormat="1" ht="128.25" x14ac:dyDescent="0.25">
       <c r="A33" s="50"/>
       <c r="B33" s="50"/>
       <c r="C33" s="51"/>
-      <c r="D33" s="44"/>
+      <c r="D33" s="48"/>
       <c r="E33" s="22" t="s">
         <v>171</v>
       </c>
@@ -3537,14 +3537,14 @@
       <c r="G33" s="22" t="s">
         <v>173</v>
       </c>
-      <c r="H33" s="42"/>
+      <c r="H33" s="45"/>
       <c r="I33" s="8"/>
     </row>
     <row r="34" spans="1:9" s="20" customFormat="1" ht="128.25" x14ac:dyDescent="0.25">
       <c r="A34" s="50"/>
       <c r="B34" s="50"/>
       <c r="C34" s="51"/>
-      <c r="D34" s="44"/>
+      <c r="D34" s="48"/>
       <c r="E34" s="22" t="s">
         <v>174</v>
       </c>
@@ -3554,14 +3554,14 @@
       <c r="G34" s="22" t="s">
         <v>176</v>
       </c>
-      <c r="H34" s="42"/>
+      <c r="H34" s="45"/>
       <c r="I34" s="19"/>
     </row>
     <row r="35" spans="1:9" s="9" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A35" s="50"/>
       <c r="B35" s="50"/>
       <c r="C35" s="51"/>
-      <c r="D35" s="44"/>
+      <c r="D35" s="48"/>
       <c r="E35" s="22" t="s">
         <v>177</v>
       </c>
@@ -3571,14 +3571,14 @@
       <c r="G35" s="22" t="s">
         <v>179</v>
       </c>
-      <c r="H35" s="42"/>
+      <c r="H35" s="45"/>
       <c r="I35" s="8"/>
     </row>
     <row r="36" spans="1:9" s="9" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A36" s="50"/>
       <c r="B36" s="50"/>
       <c r="C36" s="51"/>
-      <c r="D36" s="44"/>
+      <c r="D36" s="48"/>
       <c r="E36" s="22" t="s">
         <v>180</v>
       </c>
@@ -3588,14 +3588,14 @@
       <c r="G36" s="22" t="s">
         <v>182</v>
       </c>
-      <c r="H36" s="42"/>
+      <c r="H36" s="45"/>
       <c r="I36" s="8"/>
     </row>
     <row r="37" spans="1:9" s="9" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A37" s="50"/>
       <c r="B37" s="50"/>
       <c r="C37" s="51"/>
-      <c r="D37" s="44"/>
+      <c r="D37" s="48"/>
       <c r="E37" s="22" t="s">
         <v>183</v>
       </c>
@@ -3603,16 +3603,16 @@
         <v>184</v>
       </c>
       <c r="G37" s="22" t="s">
-        <v>302</v>
-      </c>
-      <c r="H37" s="42"/>
+        <v>301</v>
+      </c>
+      <c r="H37" s="45"/>
       <c r="I37" s="8"/>
     </row>
     <row r="38" spans="1:9" s="9" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A38" s="50"/>
       <c r="B38" s="50"/>
       <c r="C38" s="51"/>
-      <c r="D38" s="44"/>
+      <c r="D38" s="48"/>
       <c r="E38" s="22" t="s">
         <v>185</v>
       </c>
@@ -3622,14 +3622,14 @@
       <c r="G38" s="22" t="s">
         <v>187</v>
       </c>
-      <c r="H38" s="42"/>
+      <c r="H38" s="45"/>
       <c r="I38" s="8"/>
     </row>
     <row r="39" spans="1:9" s="9" customFormat="1" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A39" s="50"/>
       <c r="B39" s="50"/>
       <c r="C39" s="51"/>
-      <c r="D39" s="44"/>
+      <c r="D39" s="48"/>
       <c r="E39" s="22" t="s">
         <v>188</v>
       </c>
@@ -3637,14 +3637,14 @@
         <v>189</v>
       </c>
       <c r="G39" s="22"/>
-      <c r="H39" s="42"/>
+      <c r="H39" s="45"/>
       <c r="I39" s="8"/>
     </row>
     <row r="40" spans="1:9" s="9" customFormat="1" ht="85.5" x14ac:dyDescent="0.25">
       <c r="A40" s="50"/>
       <c r="B40" s="50"/>
       <c r="C40" s="51"/>
-      <c r="D40" s="44"/>
+      <c r="D40" s="48"/>
       <c r="E40" s="22" t="s">
         <v>190</v>
       </c>
@@ -3654,14 +3654,14 @@
       <c r="G40" s="22" t="s">
         <v>192</v>
       </c>
-      <c r="H40" s="42"/>
+      <c r="H40" s="45"/>
       <c r="I40" s="8"/>
     </row>
     <row r="41" spans="1:9" s="9" customFormat="1" ht="99.75" x14ac:dyDescent="0.25">
       <c r="A41" s="50"/>
       <c r="B41" s="50"/>
       <c r="C41" s="51"/>
-      <c r="D41" s="44"/>
+      <c r="D41" s="48"/>
       <c r="E41" s="22" t="s">
         <v>193</v>
       </c>
@@ -3671,14 +3671,14 @@
       <c r="G41" s="22" t="s">
         <v>195</v>
       </c>
-      <c r="H41" s="42"/>
+      <c r="H41" s="45"/>
       <c r="I41" s="8"/>
     </row>
     <row r="42" spans="1:9" s="9" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A42" s="50"/>
       <c r="B42" s="50"/>
       <c r="C42" s="51"/>
-      <c r="D42" s="44"/>
+      <c r="D42" s="48"/>
       <c r="E42" s="22" t="s">
         <v>196</v>
       </c>
@@ -3688,14 +3688,14 @@
       <c r="G42" s="22" t="s">
         <v>198</v>
       </c>
-      <c r="H42" s="42"/>
+      <c r="H42" s="45"/>
       <c r="I42" s="8"/>
     </row>
     <row r="43" spans="1:9" s="9" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A43" s="50"/>
       <c r="B43" s="50"/>
       <c r="C43" s="51"/>
-      <c r="D43" s="44"/>
+      <c r="D43" s="48"/>
       <c r="E43" s="22" t="s">
         <v>199</v>
       </c>
@@ -3705,14 +3705,14 @@
       <c r="G43" s="22" t="s">
         <v>201</v>
       </c>
-      <c r="H43" s="42"/>
+      <c r="H43" s="45"/>
       <c r="I43" s="8"/>
     </row>
     <row r="44" spans="1:9" s="9" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A44" s="50"/>
       <c r="B44" s="50"/>
       <c r="C44" s="51"/>
-      <c r="D44" s="44"/>
+      <c r="D44" s="48"/>
       <c r="E44" s="22" t="s">
         <v>202</v>
       </c>
@@ -3722,14 +3722,14 @@
       <c r="G44" s="22" t="s">
         <v>204</v>
       </c>
-      <c r="H44" s="42"/>
+      <c r="H44" s="45"/>
       <c r="I44" s="8"/>
     </row>
     <row r="45" spans="1:9" s="9" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A45" s="50"/>
       <c r="B45" s="50"/>
       <c r="C45" s="51"/>
-      <c r="D45" s="44"/>
+      <c r="D45" s="48"/>
       <c r="E45" s="22" t="s">
         <v>205</v>
       </c>
@@ -3739,14 +3739,14 @@
       <c r="G45" s="22" t="s">
         <v>207</v>
       </c>
-      <c r="H45" s="42"/>
+      <c r="H45" s="45"/>
       <c r="I45" s="8"/>
     </row>
     <row r="46" spans="1:9" s="9" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A46" s="50"/>
       <c r="B46" s="50"/>
       <c r="C46" s="51"/>
-      <c r="D46" s="44"/>
+      <c r="D46" s="48"/>
       <c r="E46" s="22" t="s">
         <v>208</v>
       </c>
@@ -3756,14 +3756,14 @@
       <c r="G46" s="22" t="s">
         <v>210</v>
       </c>
-      <c r="H46" s="42"/>
+      <c r="H46" s="45"/>
       <c r="I46" s="8"/>
     </row>
     <row r="47" spans="1:9" s="9" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A47" s="50"/>
       <c r="B47" s="50"/>
       <c r="C47" s="51"/>
-      <c r="D47" s="44"/>
+      <c r="D47" s="48"/>
       <c r="E47" s="22" t="s">
         <v>211</v>
       </c>
@@ -3773,14 +3773,14 @@
       <c r="G47" s="22" t="s">
         <v>213</v>
       </c>
-      <c r="H47" s="42"/>
+      <c r="H47" s="45"/>
       <c r="I47" s="8"/>
     </row>
     <row r="48" spans="1:9" s="9" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A48" s="50"/>
       <c r="B48" s="50"/>
       <c r="C48" s="51"/>
-      <c r="D48" s="44"/>
+      <c r="D48" s="48"/>
       <c r="E48" s="22" t="s">
         <v>214</v>
       </c>
@@ -3790,14 +3790,14 @@
       <c r="G48" s="22" t="s">
         <v>216</v>
       </c>
-      <c r="H48" s="42"/>
+      <c r="H48" s="45"/>
       <c r="I48" s="8"/>
     </row>
     <row r="49" spans="1:9" s="9" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A49" s="50"/>
       <c r="B49" s="50"/>
       <c r="C49" s="51"/>
-      <c r="D49" s="44"/>
+      <c r="D49" s="48"/>
       <c r="E49" s="22" t="s">
         <v>217</v>
       </c>
@@ -3807,14 +3807,14 @@
       <c r="G49" s="22" t="s">
         <v>207</v>
       </c>
-      <c r="H49" s="42"/>
+      <c r="H49" s="45"/>
       <c r="I49" s="8"/>
     </row>
     <row r="50" spans="1:9" s="9" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A50" s="50"/>
       <c r="B50" s="50"/>
       <c r="C50" s="51"/>
-      <c r="D50" s="44"/>
+      <c r="D50" s="48"/>
       <c r="E50" s="22" t="s">
         <v>219</v>
       </c>
@@ -3824,14 +3824,14 @@
       <c r="G50" s="22" t="s">
         <v>210</v>
       </c>
-      <c r="H50" s="42"/>
+      <c r="H50" s="45"/>
       <c r="I50" s="8"/>
     </row>
     <row r="51" spans="1:9" s="9" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A51" s="50"/>
       <c r="B51" s="50"/>
       <c r="C51" s="51"/>
-      <c r="D51" s="44"/>
+      <c r="D51" s="48"/>
       <c r="E51" s="22" t="s">
         <v>221</v>
       </c>
@@ -3841,14 +3841,14 @@
       <c r="G51" s="22" t="s">
         <v>223</v>
       </c>
-      <c r="H51" s="42"/>
+      <c r="H51" s="45"/>
       <c r="I51" s="8"/>
     </row>
     <row r="52" spans="1:9" s="9" customFormat="1" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="50"/>
       <c r="B52" s="50"/>
       <c r="C52" s="51"/>
-      <c r="D52" s="44"/>
+      <c r="D52" s="48"/>
       <c r="E52" s="22" t="s">
         <v>237</v>
       </c>
@@ -3858,14 +3858,14 @@
       <c r="G52" s="22" t="s">
         <v>239</v>
       </c>
-      <c r="H52" s="42"/>
+      <c r="H52" s="45"/>
       <c r="I52" s="8"/>
     </row>
     <row r="53" spans="1:9" s="9" customFormat="1" ht="299.25" x14ac:dyDescent="0.25">
       <c r="A53" s="50"/>
       <c r="B53" s="50"/>
       <c r="C53" s="51"/>
-      <c r="D53" s="44"/>
+      <c r="D53" s="48"/>
       <c r="E53" s="22" t="s">
         <v>234</v>
       </c>
@@ -3875,7 +3875,7 @@
       <c r="G53" s="22" t="s">
         <v>236</v>
       </c>
-      <c r="H53" s="42"/>
+      <c r="H53" s="45"/>
       <c r="I53" s="8"/>
     </row>
     <row r="54" spans="1:9" s="9" customFormat="1" ht="185.25" x14ac:dyDescent="0.25">
@@ -3888,17 +3888,17 @@
       <c r="C54" s="35" t="s">
         <v>102</v>
       </c>
-      <c r="D54" s="43" t="s">
+      <c r="D54" s="47" t="s">
         <v>52</v>
       </c>
       <c r="E54" s="17" t="s">
+        <v>302</v>
+      </c>
+      <c r="F54" s="17" t="s">
         <v>303</v>
       </c>
-      <c r="F54" s="17" t="s">
+      <c r="G54" s="17" t="s">
         <v>304</v>
-      </c>
-      <c r="G54" s="17" t="s">
-        <v>305</v>
       </c>
       <c r="H54" s="36" t="s">
         <v>83</v>
@@ -3906,16 +3906,16 @@
       <c r="I54" s="8"/>
     </row>
     <row r="55" spans="1:9" s="9" customFormat="1" ht="168.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="43" t="s">
+      <c r="A55" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="B55" s="43" t="s">
+      <c r="B55" s="47" t="s">
         <v>35</v>
       </c>
-      <c r="C55" s="41" t="s">
+      <c r="C55" s="44" t="s">
         <v>103</v>
       </c>
-      <c r="D55" s="44"/>
+      <c r="D55" s="48"/>
       <c r="E55" s="17" t="s">
         <v>67</v>
       </c>
@@ -3929,33 +3929,33 @@
       <c r="I55" s="8"/>
     </row>
     <row r="56" spans="1:9" s="9" customFormat="1" ht="256.5" x14ac:dyDescent="0.25">
-      <c r="A56" s="44"/>
-      <c r="B56" s="44"/>
-      <c r="C56" s="42"/>
-      <c r="D56" s="44"/>
+      <c r="A56" s="48"/>
+      <c r="B56" s="48"/>
+      <c r="C56" s="45"/>
+      <c r="D56" s="48"/>
       <c r="E56" s="17" t="s">
+        <v>305</v>
+      </c>
+      <c r="F56" s="17" t="s">
         <v>306</v>
       </c>
-      <c r="F56" s="17" t="s">
+      <c r="G56" s="17" t="s">
         <v>307</v>
-      </c>
-      <c r="G56" s="17" t="s">
-        <v>308</v>
       </c>
       <c r="H56" s="36"/>
       <c r="I56" s="8"/>
     </row>
     <row r="57" spans="1:9" s="9" customFormat="1" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="A57" s="43" t="s">
+      <c r="A57" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="B57" s="43" t="s">
+      <c r="B57" s="47" t="s">
         <v>36</v>
       </c>
-      <c r="C57" s="41" t="s">
+      <c r="C57" s="44" t="s">
         <v>104</v>
       </c>
-      <c r="D57" s="43" t="s">
+      <c r="D57" s="47" t="s">
         <v>53</v>
       </c>
       <c r="E57" s="17" t="s">
@@ -3973,27 +3973,27 @@
       <c r="I57" s="8"/>
     </row>
     <row r="58" spans="1:9" s="9" customFormat="1" ht="85.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="44"/>
-      <c r="B58" s="44"/>
-      <c r="C58" s="42"/>
-      <c r="D58" s="44"/>
+      <c r="A58" s="48"/>
+      <c r="B58" s="48"/>
+      <c r="C58" s="45"/>
+      <c r="D58" s="48"/>
       <c r="E58" s="17" t="s">
+        <v>308</v>
+      </c>
+      <c r="F58" s="17" t="s">
         <v>309</v>
       </c>
-      <c r="F58" s="17" t="s">
+      <c r="G58" s="17" t="s">
         <v>310</v>
-      </c>
-      <c r="G58" s="17" t="s">
-        <v>311</v>
       </c>
       <c r="H58" s="28"/>
       <c r="I58" s="8"/>
     </row>
     <row r="59" spans="1:9" s="9" customFormat="1" ht="85.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="44"/>
-      <c r="B59" s="44"/>
-      <c r="C59" s="42"/>
-      <c r="D59" s="44"/>
+      <c r="A59" s="48"/>
+      <c r="B59" s="48"/>
+      <c r="C59" s="45"/>
+      <c r="D59" s="48"/>
       <c r="E59" s="17" t="s">
         <v>240</v>
       </c>
@@ -4007,27 +4007,27 @@
       <c r="I59" s="8"/>
     </row>
     <row r="60" spans="1:9" s="9" customFormat="1" ht="85.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="44"/>
-      <c r="B60" s="44"/>
-      <c r="C60" s="42"/>
-      <c r="D60" s="44"/>
+      <c r="A60" s="48"/>
+      <c r="B60" s="48"/>
+      <c r="C60" s="45"/>
+      <c r="D60" s="48"/>
       <c r="E60" s="17" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="F60" s="17" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="G60" s="17"/>
       <c r="H60" s="28"/>
       <c r="I60" s="8"/>
     </row>
     <row r="61" spans="1:9" s="9" customFormat="1" ht="85.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="48"/>
-      <c r="B61" s="48"/>
-      <c r="C61" s="49"/>
-      <c r="D61" s="48"/>
+      <c r="A61" s="49"/>
+      <c r="B61" s="49"/>
+      <c r="C61" s="46"/>
+      <c r="D61" s="49"/>
       <c r="E61" s="17" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="F61" s="17" t="s">
         <v>260</v>
@@ -4046,17 +4046,17 @@
       <c r="C62" s="35" t="s">
         <v>105</v>
       </c>
-      <c r="D62" s="43" t="s">
+      <c r="D62" s="47" t="s">
         <v>54</v>
       </c>
       <c r="E62" s="17" t="s">
+        <v>311</v>
+      </c>
+      <c r="F62" s="17" t="s">
         <v>312</v>
       </c>
-      <c r="F62" s="17" t="s">
+      <c r="G62" s="17" t="s">
         <v>313</v>
-      </c>
-      <c r="G62" s="17" t="s">
-        <v>314</v>
       </c>
       <c r="H62" s="36" t="s">
         <v>85</v>
@@ -4064,16 +4064,16 @@
       <c r="I62" s="8"/>
     </row>
     <row r="63" spans="1:9" s="9" customFormat="1" ht="185.25" x14ac:dyDescent="0.25">
-      <c r="A63" s="43" t="s">
+      <c r="A63" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="B63" s="43" t="s">
+      <c r="B63" s="47" t="s">
         <v>38</v>
       </c>
-      <c r="C63" s="41" t="s">
+      <c r="C63" s="44" t="s">
         <v>132</v>
       </c>
-      <c r="D63" s="44"/>
+      <c r="D63" s="48"/>
       <c r="E63" s="17" t="s">
         <v>68</v>
       </c>
@@ -4081,33 +4081,33 @@
         <v>131</v>
       </c>
       <c r="G63" s="17" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="H63" s="25"/>
       <c r="I63" s="8"/>
     </row>
     <row r="64" spans="1:9" s="9" customFormat="1" ht="129.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="44"/>
-      <c r="B64" s="44"/>
-      <c r="C64" s="42"/>
-      <c r="D64" s="44"/>
+      <c r="A64" s="48"/>
+      <c r="B64" s="48"/>
+      <c r="C64" s="45"/>
+      <c r="D64" s="48"/>
       <c r="E64" s="17" t="s">
+        <v>315</v>
+      </c>
+      <c r="F64" s="17" t="s">
         <v>316</v>
       </c>
-      <c r="F64" s="17" t="s">
+      <c r="G64" s="17" t="s">
         <v>317</v>
-      </c>
-      <c r="G64" s="17" t="s">
-        <v>318</v>
       </c>
       <c r="H64" s="25"/>
       <c r="I64" s="8"/>
     </row>
     <row r="65" spans="1:9" s="9" customFormat="1" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="44"/>
-      <c r="B65" s="44"/>
-      <c r="C65" s="42"/>
-      <c r="D65" s="44"/>
+      <c r="A65" s="48"/>
+      <c r="B65" s="48"/>
+      <c r="C65" s="45"/>
+      <c r="D65" s="48"/>
       <c r="E65" s="17" t="s">
         <v>226</v>
       </c>
@@ -4115,55 +4115,55 @@
         <v>285</v>
       </c>
       <c r="G65" s="17" t="s">
-        <v>361</v>
+        <v>386</v>
       </c>
       <c r="H65" s="25"/>
       <c r="I65" s="8"/>
     </row>
     <row r="66" spans="1:9" s="9" customFormat="1" ht="388.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="44"/>
-      <c r="B66" s="44"/>
-      <c r="C66" s="42"/>
-      <c r="D66" s="44"/>
+      <c r="A66" s="48"/>
+      <c r="B66" s="48"/>
+      <c r="C66" s="45"/>
+      <c r="D66" s="48"/>
       <c r="E66" s="17" t="s">
+        <v>318</v>
+      </c>
+      <c r="F66" s="17" t="s">
         <v>319</v>
       </c>
-      <c r="F66" s="17" t="s">
+      <c r="G66" s="17" t="s">
         <v>320</v>
-      </c>
-      <c r="G66" s="17" t="s">
-        <v>321</v>
       </c>
       <c r="H66" s="25"/>
       <c r="I66" s="8"/>
     </row>
     <row r="67" spans="1:9" s="9" customFormat="1" ht="409.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="44"/>
-      <c r="B67" s="44"/>
-      <c r="C67" s="42"/>
-      <c r="D67" s="44"/>
+      <c r="A67" s="48"/>
+      <c r="B67" s="48"/>
+      <c r="C67" s="45"/>
+      <c r="D67" s="48"/>
       <c r="E67" s="17" t="s">
+        <v>321</v>
+      </c>
+      <c r="F67" s="17" t="s">
         <v>322</v>
       </c>
-      <c r="F67" s="17" t="s">
-        <v>323</v>
-      </c>
       <c r="G67" s="17" t="s">
-        <v>324</v>
+        <v>387</v>
       </c>
       <c r="H67" s="25"/>
       <c r="I67" s="8"/>
     </row>
     <row r="68" spans="1:9" s="9" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A68" s="48"/>
-      <c r="B68" s="48"/>
-      <c r="C68" s="49"/>
-      <c r="D68" s="48"/>
+      <c r="A68" s="49"/>
+      <c r="B68" s="49"/>
+      <c r="C68" s="46"/>
+      <c r="D68" s="49"/>
       <c r="E68" s="17" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="F68" s="17" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="G68" s="17"/>
       <c r="H68" s="25"/>
@@ -4183,28 +4183,28 @@
         <v>55</v>
       </c>
       <c r="E69" s="22" t="s">
+        <v>323</v>
+      </c>
+      <c r="F69" s="22" t="s">
+        <v>324</v>
+      </c>
+      <c r="G69" s="22" t="s">
         <v>325</v>
-      </c>
-      <c r="F69" s="22" t="s">
-        <v>326</v>
-      </c>
-      <c r="G69" s="22" t="s">
-        <v>327</v>
       </c>
       <c r="H69" s="26"/>
       <c r="I69" s="8"/>
     </row>
     <row r="70" spans="1:9" s="9" customFormat="1" ht="58.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="56" t="s">
+      <c r="A70" s="53" t="s">
         <v>24</v>
       </c>
-      <c r="B70" s="56" t="s">
+      <c r="B70" s="53" t="s">
         <v>40</v>
       </c>
-      <c r="C70" s="45" t="s">
+      <c r="C70" s="57" t="s">
         <v>134</v>
       </c>
-      <c r="D70" s="56" t="s">
+      <c r="D70" s="53" t="s">
         <v>53</v>
       </c>
       <c r="E70" s="17" t="s">
@@ -4220,27 +4220,27 @@
       <c r="I70" s="8"/>
     </row>
     <row r="71" spans="1:9" s="9" customFormat="1" ht="58.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="57"/>
-      <c r="B71" s="57"/>
-      <c r="C71" s="46"/>
-      <c r="D71" s="57"/>
+      <c r="A71" s="54"/>
+      <c r="B71" s="54"/>
+      <c r="C71" s="58"/>
+      <c r="D71" s="54"/>
       <c r="E71" s="17" t="s">
+        <v>308</v>
+      </c>
+      <c r="F71" s="17" t="s">
         <v>309</v>
       </c>
-      <c r="F71" s="17" t="s">
+      <c r="G71" s="17" t="s">
         <v>310</v>
-      </c>
-      <c r="G71" s="17" t="s">
-        <v>311</v>
       </c>
       <c r="H71" s="26"/>
       <c r="I71" s="8"/>
     </row>
     <row r="72" spans="1:9" s="9" customFormat="1" ht="58.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="57"/>
-      <c r="B72" s="57"/>
-      <c r="C72" s="46"/>
-      <c r="D72" s="57"/>
+      <c r="A72" s="54"/>
+      <c r="B72" s="54"/>
+      <c r="C72" s="58"/>
+      <c r="D72" s="54"/>
       <c r="E72" s="17" t="s">
         <v>240</v>
       </c>
@@ -4254,27 +4254,27 @@
       <c r="I72" s="8"/>
     </row>
     <row r="73" spans="1:9" s="9" customFormat="1" ht="58.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="57"/>
-      <c r="B73" s="57"/>
-      <c r="C73" s="46"/>
-      <c r="D73" s="57"/>
+      <c r="A73" s="54"/>
+      <c r="B73" s="54"/>
+      <c r="C73" s="58"/>
+      <c r="D73" s="54"/>
       <c r="E73" s="17" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="F73" s="17" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="G73" s="17"/>
       <c r="H73" s="26"/>
       <c r="I73" s="8"/>
     </row>
     <row r="74" spans="1:9" s="9" customFormat="1" ht="58.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="58"/>
-      <c r="B74" s="58"/>
-      <c r="C74" s="47"/>
-      <c r="D74" s="58"/>
+      <c r="A74" s="55"/>
+      <c r="B74" s="55"/>
+      <c r="C74" s="59"/>
+      <c r="D74" s="55"/>
       <c r="E74" s="17" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="F74" s="17" t="s">
         <v>260</v>
@@ -4297,13 +4297,13 @@
         <v>57</v>
       </c>
       <c r="E75" s="17" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="F75" s="17" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="G75" s="17" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="H75" s="36"/>
       <c r="I75" s="8"/>
@@ -4318,7 +4318,7 @@
       <c r="C76" s="35" t="s">
         <v>136</v>
       </c>
-      <c r="D76" s="55" t="s">
+      <c r="D76" s="52" t="s">
         <v>58</v>
       </c>
       <c r="E76" s="22" t="s">
@@ -4341,7 +4341,7 @@
       <c r="C77" s="35" t="s">
         <v>107</v>
       </c>
-      <c r="D77" s="55"/>
+      <c r="D77" s="52"/>
       <c r="E77" s="22" t="s">
         <v>245</v>
       </c>
@@ -4362,13 +4362,13 @@
       <c r="C78" s="35" t="s">
         <v>137</v>
       </c>
-      <c r="D78" s="43" t="s">
+      <c r="D78" s="47" t="s">
         <v>59</v>
       </c>
       <c r="E78" s="25"/>
       <c r="F78" s="25"/>
       <c r="G78" s="25"/>
-      <c r="H78" s="55" t="s">
+      <c r="H78" s="52" t="s">
         <v>86</v>
       </c>
       <c r="I78" s="8"/>
@@ -4383,94 +4383,94 @@
       <c r="C79" s="35" t="s">
         <v>108</v>
       </c>
-      <c r="D79" s="48"/>
+      <c r="D79" s="49"/>
       <c r="E79" s="30"/>
       <c r="F79" s="29"/>
       <c r="G79" s="29"/>
-      <c r="H79" s="55"/>
+      <c r="H79" s="52"/>
       <c r="I79" s="8"/>
     </row>
     <row r="80" spans="1:9" s="9" customFormat="1" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="43" t="s">
+      <c r="A80" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="B80" s="43" t="s">
+      <c r="B80" s="47" t="s">
         <v>46</v>
       </c>
-      <c r="C80" s="41" t="s">
+      <c r="C80" s="44" t="s">
         <v>138</v>
       </c>
-      <c r="D80" s="43" t="s">
-        <v>329</v>
+      <c r="D80" s="47" t="s">
+        <v>327</v>
       </c>
       <c r="E80" s="17" t="s">
+        <v>349</v>
+      </c>
+      <c r="F80" s="17" t="s">
+        <v>350</v>
+      </c>
+      <c r="G80" s="17" t="s">
         <v>351</v>
       </c>
-      <c r="F80" s="17" t="s">
-        <v>352</v>
-      </c>
-      <c r="G80" s="17" t="s">
-        <v>353</v>
-      </c>
-      <c r="H80" s="55"/>
+      <c r="H80" s="52"/>
       <c r="I80" s="8"/>
     </row>
     <row r="81" spans="1:9" s="9" customFormat="1" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="A81" s="44"/>
-      <c r="B81" s="44"/>
-      <c r="C81" s="42"/>
-      <c r="D81" s="44"/>
+      <c r="A81" s="48"/>
+      <c r="B81" s="48"/>
+      <c r="C81" s="45"/>
+      <c r="D81" s="48"/>
       <c r="E81" s="17" t="s">
+        <v>346</v>
+      </c>
+      <c r="F81" s="17" t="s">
+        <v>347</v>
+      </c>
+      <c r="G81" s="17" t="s">
         <v>348</v>
-      </c>
-      <c r="F81" s="17" t="s">
-        <v>349</v>
-      </c>
-      <c r="G81" s="17" t="s">
-        <v>350</v>
       </c>
       <c r="H81" s="27"/>
       <c r="I81" s="8"/>
     </row>
     <row r="82" spans="1:9" s="9" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A82" s="44"/>
-      <c r="B82" s="44"/>
-      <c r="C82" s="42"/>
-      <c r="D82" s="44"/>
+      <c r="A82" s="48"/>
+      <c r="B82" s="48"/>
+      <c r="C82" s="45"/>
+      <c r="D82" s="48"/>
       <c r="E82" s="17" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="F82" s="17" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="G82" s="17" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="H82" s="27"/>
       <c r="I82" s="8"/>
     </row>
     <row r="83" spans="1:9" s="9" customFormat="1" ht="57" x14ac:dyDescent="0.25">
-      <c r="A83" s="44"/>
-      <c r="B83" s="44"/>
-      <c r="C83" s="42"/>
-      <c r="D83" s="44"/>
+      <c r="A83" s="48"/>
+      <c r="B83" s="48"/>
+      <c r="C83" s="45"/>
+      <c r="D83" s="48"/>
       <c r="E83" s="17" t="s">
+        <v>342</v>
+      </c>
+      <c r="F83" s="17" t="s">
+        <v>343</v>
+      </c>
+      <c r="G83" s="17" t="s">
         <v>344</v>
-      </c>
-      <c r="F83" s="17" t="s">
-        <v>345</v>
-      </c>
-      <c r="G83" s="17" t="s">
-        <v>346</v>
       </c>
       <c r="H83" s="27"/>
       <c r="I83" s="8"/>
     </row>
     <row r="84" spans="1:9" s="9" customFormat="1" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="A84" s="44"/>
-      <c r="B84" s="44"/>
-      <c r="C84" s="42"/>
-      <c r="D84" s="44"/>
+      <c r="A84" s="48"/>
+      <c r="B84" s="48"/>
+      <c r="C84" s="45"/>
+      <c r="D84" s="48"/>
       <c r="E84" s="17" t="s">
         <v>286</v>
       </c>
@@ -4484,78 +4484,78 @@
       <c r="I84" s="8"/>
     </row>
     <row r="85" spans="1:9" s="9" customFormat="1" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="A85" s="44"/>
-      <c r="B85" s="44"/>
-      <c r="C85" s="42"/>
-      <c r="D85" s="44"/>
+      <c r="A85" s="48"/>
+      <c r="B85" s="48"/>
+      <c r="C85" s="45"/>
+      <c r="D85" s="48"/>
       <c r="E85" s="17" t="s">
+        <v>339</v>
+      </c>
+      <c r="F85" s="17" t="s">
+        <v>340</v>
+      </c>
+      <c r="G85" s="17" t="s">
         <v>341</v>
-      </c>
-      <c r="F85" s="17" t="s">
-        <v>342</v>
-      </c>
-      <c r="G85" s="17" t="s">
-        <v>343</v>
       </c>
       <c r="H85" s="27"/>
       <c r="I85" s="8"/>
     </row>
     <row r="86" spans="1:9" s="9" customFormat="1" ht="57" x14ac:dyDescent="0.25">
-      <c r="A86" s="44"/>
-      <c r="B86" s="44"/>
-      <c r="C86" s="42"/>
-      <c r="D86" s="44"/>
+      <c r="A86" s="48"/>
+      <c r="B86" s="48"/>
+      <c r="C86" s="45"/>
+      <c r="D86" s="48"/>
       <c r="E86" s="17" t="s">
         <v>289</v>
       </c>
       <c r="F86" s="17" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="G86" s="17" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="H86" s="27"/>
       <c r="I86" s="8"/>
     </row>
     <row r="87" spans="1:9" s="9" customFormat="1" ht="114" x14ac:dyDescent="0.25">
-      <c r="A87" s="44"/>
-      <c r="B87" s="44"/>
-      <c r="C87" s="42"/>
-      <c r="D87" s="44"/>
+      <c r="A87" s="48"/>
+      <c r="B87" s="48"/>
+      <c r="C87" s="45"/>
+      <c r="D87" s="48"/>
       <c r="E87" s="17" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="F87" s="17" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="G87" s="17" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="H87" s="27"/>
       <c r="I87" s="8"/>
     </row>
     <row r="88" spans="1:9" s="9" customFormat="1" ht="99.75" x14ac:dyDescent="0.25">
-      <c r="A88" s="44"/>
-      <c r="B88" s="44"/>
-      <c r="C88" s="42"/>
-      <c r="D88" s="44"/>
+      <c r="A88" s="48"/>
+      <c r="B88" s="48"/>
+      <c r="C88" s="45"/>
+      <c r="D88" s="48"/>
       <c r="E88" s="17" t="s">
+        <v>332</v>
+      </c>
+      <c r="F88" s="17" t="s">
+        <v>333</v>
+      </c>
+      <c r="G88" s="17" t="s">
         <v>334</v>
-      </c>
-      <c r="F88" s="17" t="s">
-        <v>335</v>
-      </c>
-      <c r="G88" s="17" t="s">
-        <v>336</v>
       </c>
       <c r="H88" s="27"/>
       <c r="I88" s="8"/>
     </row>
     <row r="89" spans="1:9" s="9" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A89" s="44"/>
-      <c r="B89" s="44"/>
-      <c r="C89" s="42"/>
-      <c r="D89" s="44"/>
+      <c r="A89" s="48"/>
+      <c r="B89" s="48"/>
+      <c r="C89" s="45"/>
+      <c r="D89" s="48"/>
       <c r="E89" s="17" t="s">
         <v>264</v>
       </c>
@@ -4569,10 +4569,10 @@
       <c r="I89" s="8"/>
     </row>
     <row r="90" spans="1:9" s="9" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A90" s="44"/>
-      <c r="B90" s="44"/>
-      <c r="C90" s="42"/>
-      <c r="D90" s="44"/>
+      <c r="A90" s="48"/>
+      <c r="B90" s="48"/>
+      <c r="C90" s="45"/>
+      <c r="D90" s="48"/>
       <c r="E90" s="17" t="s">
         <v>267</v>
       </c>
@@ -4586,10 +4586,10 @@
       <c r="I90" s="8"/>
     </row>
     <row r="91" spans="1:9" s="9" customFormat="1" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="A91" s="44"/>
-      <c r="B91" s="44"/>
-      <c r="C91" s="42"/>
-      <c r="D91" s="44"/>
+      <c r="A91" s="48"/>
+      <c r="B91" s="48"/>
+      <c r="C91" s="45"/>
+      <c r="D91" s="48"/>
       <c r="E91" s="17" t="s">
         <v>270</v>
       </c>
@@ -4603,10 +4603,10 @@
       <c r="I91" s="8"/>
     </row>
     <row r="92" spans="1:9" s="9" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A92" s="44"/>
-      <c r="B92" s="44"/>
-      <c r="C92" s="42"/>
-      <c r="D92" s="44"/>
+      <c r="A92" s="48"/>
+      <c r="B92" s="48"/>
+      <c r="C92" s="45"/>
+      <c r="D92" s="48"/>
       <c r="E92" s="17" t="s">
         <v>273</v>
       </c>
@@ -4620,10 +4620,10 @@
       <c r="I92" s="8"/>
     </row>
     <row r="93" spans="1:9" s="9" customFormat="1" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="A93" s="44"/>
-      <c r="B93" s="44"/>
-      <c r="C93" s="42"/>
-      <c r="D93" s="44"/>
+      <c r="A93" s="48"/>
+      <c r="B93" s="48"/>
+      <c r="C93" s="45"/>
+      <c r="D93" s="48"/>
       <c r="E93" s="17" t="s">
         <v>276</v>
       </c>
@@ -4637,10 +4637,10 @@
       <c r="I93" s="8"/>
     </row>
     <row r="94" spans="1:9" s="9" customFormat="1" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="A94" s="44"/>
-      <c r="B94" s="44"/>
-      <c r="C94" s="42"/>
-      <c r="D94" s="44"/>
+      <c r="A94" s="48"/>
+      <c r="B94" s="48"/>
+      <c r="C94" s="45"/>
+      <c r="D94" s="48"/>
       <c r="E94" s="17" t="s">
         <v>279</v>
       </c>
@@ -4654,10 +4654,10 @@
       <c r="I94" s="8"/>
     </row>
     <row r="95" spans="1:9" s="9" customFormat="1" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="A95" s="44"/>
-      <c r="B95" s="44"/>
-      <c r="C95" s="42"/>
-      <c r="D95" s="44"/>
+      <c r="A95" s="48"/>
+      <c r="B95" s="48"/>
+      <c r="C95" s="45"/>
+      <c r="D95" s="48"/>
       <c r="E95" s="17" t="s">
         <v>282</v>
       </c>
@@ -4671,10 +4671,10 @@
       <c r="I95" s="8"/>
     </row>
     <row r="96" spans="1:9" s="9" customFormat="1" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="A96" s="44"/>
-      <c r="B96" s="44"/>
-      <c r="C96" s="42"/>
-      <c r="D96" s="44"/>
+      <c r="A96" s="48"/>
+      <c r="B96" s="48"/>
+      <c r="C96" s="45"/>
+      <c r="D96" s="48"/>
       <c r="E96" s="17" t="s">
         <v>247</v>
       </c>
@@ -4688,10 +4688,10 @@
       <c r="I96" s="8"/>
     </row>
     <row r="97" spans="1:9" s="9" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A97" s="44"/>
-      <c r="B97" s="44"/>
-      <c r="C97" s="42"/>
-      <c r="D97" s="44"/>
+      <c r="A97" s="48"/>
+      <c r="B97" s="48"/>
+      <c r="C97" s="45"/>
+      <c r="D97" s="48"/>
       <c r="E97" s="17" t="s">
         <v>250</v>
       </c>
@@ -4705,27 +4705,27 @@
       <c r="I97" s="8"/>
     </row>
     <row r="98" spans="1:9" s="9" customFormat="1" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="A98" s="44"/>
-      <c r="B98" s="44"/>
-      <c r="C98" s="42"/>
-      <c r="D98" s="44"/>
+      <c r="A98" s="48"/>
+      <c r="B98" s="48"/>
+      <c r="C98" s="45"/>
+      <c r="D98" s="48"/>
       <c r="E98" s="17" t="s">
+        <v>329</v>
+      </c>
+      <c r="F98" s="17" t="s">
+        <v>330</v>
+      </c>
+      <c r="G98" s="17" t="s">
         <v>331</v>
-      </c>
-      <c r="F98" s="17" t="s">
-        <v>332</v>
-      </c>
-      <c r="G98" s="17" t="s">
-        <v>333</v>
       </c>
       <c r="H98" s="27"/>
       <c r="I98" s="8"/>
     </row>
     <row r="99" spans="1:9" s="9" customFormat="1" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="A99" s="44"/>
-      <c r="B99" s="44"/>
-      <c r="C99" s="42"/>
-      <c r="D99" s="44"/>
+      <c r="A99" s="48"/>
+      <c r="B99" s="48"/>
+      <c r="C99" s="45"/>
+      <c r="D99" s="48"/>
       <c r="E99" s="17" t="s">
         <v>253</v>
       </c>
@@ -4739,10 +4739,10 @@
       <c r="I99" s="8"/>
     </row>
     <row r="100" spans="1:9" s="9" customFormat="1" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="A100" s="44"/>
-      <c r="B100" s="44"/>
-      <c r="C100" s="42"/>
-      <c r="D100" s="44"/>
+      <c r="A100" s="48"/>
+      <c r="B100" s="48"/>
+      <c r="C100" s="45"/>
+      <c r="D100" s="48"/>
       <c r="E100" s="17" t="s">
         <v>256</v>
       </c>
@@ -4756,10 +4756,10 @@
       <c r="I100" s="8"/>
     </row>
     <row r="101" spans="1:9" s="9" customFormat="1" ht="102" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="44"/>
-      <c r="B101" s="44"/>
-      <c r="C101" s="42"/>
-      <c r="D101" s="44"/>
+      <c r="A101" s="48"/>
+      <c r="B101" s="48"/>
+      <c r="C101" s="45"/>
+      <c r="D101" s="48"/>
       <c r="E101" s="17" t="s">
         <v>259</v>
       </c>
@@ -4773,15 +4773,15 @@
       <c r="I101" s="8"/>
     </row>
     <row r="102" spans="1:9" s="9" customFormat="1" ht="102" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="44"/>
-      <c r="B102" s="44"/>
-      <c r="C102" s="42"/>
-      <c r="D102" s="44"/>
+      <c r="A102" s="48"/>
+      <c r="B102" s="48"/>
+      <c r="C102" s="45"/>
+      <c r="D102" s="48"/>
       <c r="E102" s="17" t="s">
         <v>262</v>
       </c>
       <c r="F102" s="17" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="G102" s="17" t="s">
         <v>263</v>
@@ -4799,45 +4799,45 @@
       <c r="C103" s="35" t="s">
         <v>139</v>
       </c>
-      <c r="D103" s="43" t="s">
+      <c r="D103" s="47" t="s">
         <v>60</v>
       </c>
       <c r="E103" s="17" t="s">
         <v>72</v>
       </c>
       <c r="F103" s="17" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="G103" s="17" t="s">
-        <v>370</v>
-      </c>
-      <c r="H103" s="53" t="s">
+        <v>388</v>
+      </c>
+      <c r="H103" s="41" t="s">
         <v>87</v>
       </c>
       <c r="I103" s="8"/>
     </row>
     <row r="104" spans="1:9" s="9" customFormat="1" ht="72" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="43" t="s">
+      <c r="A104" s="47" t="s">
         <v>32</v>
       </c>
-      <c r="B104" s="43" t="s">
+      <c r="B104" s="47" t="s">
         <v>48</v>
       </c>
-      <c r="C104" s="41" t="s">
+      <c r="C104" s="44" t="s">
         <v>106</v>
       </c>
-      <c r="D104" s="44"/>
+      <c r="D104" s="48"/>
       <c r="E104" s="17"/>
       <c r="F104" s="17"/>
       <c r="G104" s="17"/>
-      <c r="H104" s="54"/>
+      <c r="H104" s="42"/>
       <c r="I104" s="8"/>
     </row>
     <row r="105" spans="1:9" s="9" customFormat="1" ht="270.75" x14ac:dyDescent="0.25">
-      <c r="A105" s="44"/>
-      <c r="B105" s="44"/>
-      <c r="C105" s="42"/>
-      <c r="D105" s="44"/>
+      <c r="A105" s="48"/>
+      <c r="B105" s="48"/>
+      <c r="C105" s="45"/>
+      <c r="D105" s="48"/>
       <c r="E105" s="17" t="s">
         <v>231</v>
       </c>
@@ -4851,18 +4851,18 @@
       <c r="I105" s="8"/>
     </row>
     <row r="106" spans="1:9" s="9" customFormat="1" ht="57" x14ac:dyDescent="0.25">
-      <c r="A106" s="48"/>
-      <c r="B106" s="48"/>
-      <c r="C106" s="49"/>
-      <c r="D106" s="48"/>
+      <c r="A106" s="49"/>
+      <c r="B106" s="49"/>
+      <c r="C106" s="46"/>
+      <c r="D106" s="49"/>
       <c r="E106" s="17" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="F106" s="17" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="G106" s="17" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="H106" s="37"/>
       <c r="I106" s="8"/>
@@ -4883,11 +4883,11 @@
       <c r="E107" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="F107" s="38" t="s">
+      <c r="F107" s="22" t="s">
         <v>141</v>
       </c>
       <c r="G107" s="38" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="H107" s="21" t="s">
         <v>88</v>
@@ -4903,16 +4903,16 @@
       </c>
       <c r="C108" s="10"/>
       <c r="D108" s="21" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="E108" s="17" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="F108" s="17" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="G108" s="17" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">
@@ -4929,9 +4929,9 @@
   <sheetProtection selectLockedCells="1" autoFilter="0"/>
   <autoFilter ref="A2:H107"/>
   <customSheetViews>
-    <customSheetView guid="{265E3820-1829-4A54-B10C-5E3DB0A2FE40}" fitToPage="1">
-      <pane ySplit="2" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C17" sqref="C17"/>
+    <customSheetView guid="{64356ACC-46E0-4594-A667-8B3867E089EA}" fitToPage="1" topLeftCell="C1">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
       <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.5" header="0.5" footer="0.25"/>
       <printOptions horizontalCentered="1" verticalCentered="1"/>
       <pageSetup scale="58" fitToHeight="0" orientation="landscape" r:id="rId1"/>
@@ -4939,9 +4939,9 @@
         <oddFooter>&amp;R&amp;P of &amp;N</oddFooter>
       </headerFooter>
     </customSheetView>
-    <customSheetView guid="{64356ACC-46E0-4594-A667-8B3867E089EA}" fitToPage="1" topLeftCell="C1">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
+    <customSheetView guid="{265E3820-1829-4A54-B10C-5E3DB0A2FE40}" fitToPage="1">
+      <pane ySplit="2" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C17" sqref="C17"/>
       <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.5" header="0.5" footer="0.25"/>
       <printOptions horizontalCentered="1" verticalCentered="1"/>
       <pageSetup scale="58" fitToHeight="0" orientation="landscape" r:id="rId2"/>
@@ -4951,6 +4951,42 @@
     </customSheetView>
   </customSheetViews>
   <mergeCells count="52">
+    <mergeCell ref="B80:B102"/>
+    <mergeCell ref="A80:A102"/>
+    <mergeCell ref="C70:C74"/>
+    <mergeCell ref="D3:D6"/>
+    <mergeCell ref="A3:A6"/>
+    <mergeCell ref="B3:B6"/>
+    <mergeCell ref="C3:C6"/>
+    <mergeCell ref="D12:D18"/>
+    <mergeCell ref="D7:D11"/>
+    <mergeCell ref="C28:C53"/>
+    <mergeCell ref="D54:D56"/>
+    <mergeCell ref="A7:A11"/>
+    <mergeCell ref="B7:B11"/>
+    <mergeCell ref="C7:C11"/>
+    <mergeCell ref="A12:A21"/>
+    <mergeCell ref="D78:D79"/>
+    <mergeCell ref="A104:A106"/>
+    <mergeCell ref="D24:D27"/>
+    <mergeCell ref="D103:D106"/>
+    <mergeCell ref="C104:C106"/>
+    <mergeCell ref="B104:B106"/>
+    <mergeCell ref="A22:A27"/>
+    <mergeCell ref="C55:C56"/>
+    <mergeCell ref="B55:B56"/>
+    <mergeCell ref="C22:C27"/>
+    <mergeCell ref="B22:B27"/>
+    <mergeCell ref="A55:A56"/>
+    <mergeCell ref="D80:D102"/>
+    <mergeCell ref="A57:A61"/>
+    <mergeCell ref="A70:A74"/>
+    <mergeCell ref="C80:C102"/>
+    <mergeCell ref="H28:H53"/>
+    <mergeCell ref="D57:D61"/>
+    <mergeCell ref="D28:D53"/>
+    <mergeCell ref="D70:D74"/>
+    <mergeCell ref="B70:B74"/>
     <mergeCell ref="H103:H104"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="C63:C68"/>
@@ -4967,42 +5003,6 @@
     <mergeCell ref="D22:D23"/>
     <mergeCell ref="D19:D21"/>
     <mergeCell ref="D62:D68"/>
-    <mergeCell ref="H28:H53"/>
-    <mergeCell ref="D57:D61"/>
-    <mergeCell ref="D28:D53"/>
-    <mergeCell ref="D70:D74"/>
-    <mergeCell ref="B70:B74"/>
-    <mergeCell ref="D78:D79"/>
-    <mergeCell ref="A104:A106"/>
-    <mergeCell ref="D24:D27"/>
-    <mergeCell ref="D103:D106"/>
-    <mergeCell ref="C104:C106"/>
-    <mergeCell ref="B104:B106"/>
-    <mergeCell ref="A22:A27"/>
-    <mergeCell ref="C55:C56"/>
-    <mergeCell ref="B55:B56"/>
-    <mergeCell ref="C22:C27"/>
-    <mergeCell ref="B22:B27"/>
-    <mergeCell ref="A55:A56"/>
-    <mergeCell ref="D80:D102"/>
-    <mergeCell ref="A57:A61"/>
-    <mergeCell ref="A70:A74"/>
-    <mergeCell ref="C80:C102"/>
-    <mergeCell ref="B80:B102"/>
-    <mergeCell ref="A80:A102"/>
-    <mergeCell ref="C70:C74"/>
-    <mergeCell ref="D3:D6"/>
-    <mergeCell ref="A3:A6"/>
-    <mergeCell ref="B3:B6"/>
-    <mergeCell ref="C3:C6"/>
-    <mergeCell ref="D12:D18"/>
-    <mergeCell ref="D7:D11"/>
-    <mergeCell ref="C28:C53"/>
-    <mergeCell ref="D54:D56"/>
-    <mergeCell ref="A7:A11"/>
-    <mergeCell ref="B7:B11"/>
-    <mergeCell ref="C7:C11"/>
-    <mergeCell ref="A12:A21"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.5" header="0.5" footer="0.25"/>

</xml_diff>